<commit_message>
Update App_Christoph & Zeiterfassung_Gesamt Summenfehler behoben
Zusätzlich: Zeitbuchungen nachgeholt
</commit_message>
<xml_diff>
--- a/Dokumente/Zeiterfassung/Huber.xlsx
+++ b/Dokumente/Zeiterfassung/Huber.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomic\Documents\GitHub\259035_SoftEngPR-Base\Dokumente\Zeiterfassung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\GitHub\259035_SoftEngPR\Dokumente\Zeiterfassung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{13581AE0-8C98-45FC-B287-F430F8E63407}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13032" yWindow="0" windowWidth="18276" windowHeight="7908" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13965" yWindow="0" windowWidth="18270" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Huber" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="70">
   <si>
     <t>GESAMT</t>
   </si>
@@ -133,15 +132,117 @@
   </si>
   <si>
     <t>SQL Verbindung und Variablenanpassung</t>
+  </si>
+  <si>
+    <t>Recherche</t>
+  </si>
+  <si>
+    <t>Onlinestudium der Möglichkeiten der Graphischen Verbesserung des RC2</t>
+  </si>
+  <si>
+    <t>Designarbeiten</t>
+  </si>
+  <si>
+    <t>Beginn der Arbeit mit dem JavaFX SceneBuilder, Entwurf der ersten Scenes (Projects)</t>
+  </si>
+  <si>
+    <t>Verbesserung des Entwurfs, erstellen weiterer Scenes</t>
+  </si>
+  <si>
+    <t>Entwurf der DashboardScene, der Task Management Scene, der PopupScenes</t>
+  </si>
+  <si>
+    <t>Entwurf der userManagementScene, weitere Arbeit bei dem PopupScenes</t>
+  </si>
+  <si>
+    <t>Entwurf der restlichen Scenes, Layoutanpassungen, Hinzufügen neuer Elemente.</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Designtests</t>
+  </si>
+  <si>
+    <t>Tests der erstellen Layouts, verknüpfung erstellt bei sämtlichen Buttons, Designentwürfe getestet</t>
+  </si>
+  <si>
+    <t>Entwicklung</t>
+  </si>
+  <si>
+    <t>Verknüpfung sämtlicher "Scenes" mit den Stages, erste Versuche der Migration</t>
+  </si>
+  <si>
+    <t>Überarbeitung der Datenbankverbindung, Onlinerecherche über Hibernate</t>
+  </si>
+  <si>
+    <t>Testen einer Basishibernateklasse, Erstellen der ersten Annotations, Überarbeitung der Datenbanktabellen</t>
+  </si>
+  <si>
+    <t>Hibernatemigration vervollständigt, Tests der CRUD Operationen, Annotionen finalisiert</t>
+  </si>
+  <si>
+    <t>Designanpassung</t>
+  </si>
+  <si>
+    <t>Erstellen des LoginFensters, Erstellen der Notification und ChoiceBox, Tests</t>
+  </si>
+  <si>
+    <t>Entwicklung der Loginfunktionalität, Einführung der BusinessRoleklasse, erste Userpermissions umgesetzt</t>
+  </si>
+  <si>
+    <t>Elemente des Dashboards fertiggestellt, Tabellenmethoden geschrieben</t>
+  </si>
+  <si>
+    <t>Elemente des Usermanagement, AddUser und Edituser mit der vorgesegehen Funktionalität versehen</t>
+  </si>
+  <si>
+    <t>Erstellung der LoadDependences Klasse, Überarbeitung des "LoadScene" Verhaltens</t>
+  </si>
+  <si>
+    <t>Umbau sämtlicher Klassen von Statischen in Dynamische</t>
+  </si>
+  <si>
+    <t>Layoutfehlerbehebungen, wurde bei der erstmaligen Ausführung auf einem Laptop bemerkt</t>
+  </si>
+  <si>
+    <t>Fertigstellung der ProjectsScene, inklusive der Edit/AddProjectScenes</t>
+  </si>
+  <si>
+    <t>Erstellung des Klasse ProjectDashboardControl, inklusive der Dynamischen Tabellen</t>
+  </si>
+  <si>
+    <t>Erstellung der Klasse TaskDashboardControl</t>
+  </si>
+  <si>
+    <t>Zwischentests der bereits realisierten Funktionalität</t>
+  </si>
+  <si>
+    <t>Erstellung der ersten Reports, BarChart Projectoverview, inklusive Fehlerbehebungen</t>
+  </si>
+  <si>
+    <t>Weitere Arbeiten an den Reports, diverse Feinanpassungen, NPE Fehlerbehebungen,..</t>
+  </si>
+  <si>
+    <t>Erstellung von DemoDaten, um die Funktionalität zu testen</t>
+  </si>
+  <si>
+    <t>Abschluss</t>
+  </si>
+  <si>
+    <t>Erstellung eines weiteren Charts, anpassung der Funktionalität des Activitycharts</t>
+  </si>
+  <si>
+    <t>Finale Tests, Sicherung der Datenbank, kleinere Feinabstimmungen, CodeOverview</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="hh:mm;@"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="hh:mm;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -241,12 +342,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -260,7 +361,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -296,7 +397,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
@@ -304,8 +405,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -367,21 +468,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle36" displayName="Tabelle36" ref="B6:H51" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="B6:H51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle36" displayName="Tabelle36" ref="B6:H67" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="B6:H67"/>
   <sortState ref="B7:H44">
     <sortCondition ref="D6:D44"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Art" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Beschreibung" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Datum" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="von" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="bis" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Dauer" dataDxfId="1">
+    <tableColumn id="2" name="Art" dataDxfId="6"/>
+    <tableColumn id="3" name="Beschreibung" dataDxfId="5"/>
+    <tableColumn id="8" name="Datum" dataDxfId="4"/>
+    <tableColumn id="4" name="von" dataDxfId="3"/>
+    <tableColumn id="5" name="bis" dataDxfId="2"/>
+    <tableColumn id="15" name="Dauer" dataDxfId="1">
       <calculatedColumnFormula>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="KW" dataDxfId="0">
+    <tableColumn id="1" name="KW" dataDxfId="0">
       <calculatedColumnFormula>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -651,42 +752,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H229"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="75.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" style="1"/>
-    <col min="7" max="7" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.88671875" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="75.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="1"/>
+    <col min="7" max="7" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="25" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="24"/>
     </row>
-    <row r="3" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B3" s="25"/>
       <c r="C3" s="24"/>
     </row>
-    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="22"/>
     </row>
-    <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
         <v>15</v>
       </c>
@@ -709,7 +810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>2</v>
       </c>
@@ -734,7 +835,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>2</v>
       </c>
@@ -759,7 +860,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="15" t="s">
         <v>2</v>
@@ -785,7 +886,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>2</v>
       </c>
@@ -810,7 +911,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
         <v>2</v>
       </c>
@@ -835,7 +936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
         <v>6</v>
       </c>
@@ -860,7 +961,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="15" t="s">
         <v>2</v>
       </c>
@@ -885,7 +986,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="15" t="s">
         <v>2</v>
       </c>
@@ -910,7 +1011,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
         <v>2</v>
       </c>
@@ -935,7 +1036,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
         <v>2</v>
       </c>
@@ -960,7 +1061,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="15" t="s">
         <v>2</v>
       </c>
@@ -985,7 +1086,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="15" t="s">
         <v>2</v>
       </c>
@@ -1010,7 +1111,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
         <v>2</v>
       </c>
@@ -1035,7 +1136,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="17" t="s">
         <v>2</v>
       </c>
@@ -1060,7 +1161,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>2</v>
       </c>
@@ -1085,7 +1186,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
         <v>2</v>
       </c>
@@ -1110,7 +1211,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>2</v>
       </c>
@@ -1135,7 +1236,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>26</v>
       </c>
@@ -1160,7 +1261,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1185,7 +1286,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="14" t="s">
         <v>2</v>
       </c>
@@ -1210,7 +1311,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
         <v>30</v>
       </c>
@@ -1235,7 +1336,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="14" t="s">
         <v>2</v>
       </c>
@@ -1260,7 +1361,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
         <v>2</v>
       </c>
@@ -1285,7 +1386,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
         <v>2</v>
       </c>
@@ -1310,7 +1411,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="14" t="s">
         <v>34</v>
       </c>
@@ -1335,7 +1436,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
         <v>2</v>
       </c>
@@ -1360,478 +1461,868 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="13">
+        <v>43256</v>
+      </c>
+      <c r="E33" s="12">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F33" s="12">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="G33" s="1">
         <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>3</v>
+      </c>
+      <c r="H33" s="1">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="13">
+        <v>43258</v>
+      </c>
+      <c r="E34" s="12">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F34" s="12">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="G34" s="1">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>5</v>
+      </c>
+      <c r="H34" s="1">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="13">
+        <v>43260</v>
+      </c>
+      <c r="E35" s="12">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F35" s="12">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="G35" s="1">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>6</v>
+      </c>
+      <c r="H35" s="1">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="13">
+        <v>43261</v>
+      </c>
+      <c r="E36" s="12">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F36" s="12">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="G36" s="1">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>8</v>
+      </c>
+      <c r="H36" s="1">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="13">
+        <v>43262</v>
+      </c>
+      <c r="E37" s="12">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F37" s="12">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="G37" s="1">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>4.5</v>
+      </c>
+      <c r="H37" s="1">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="13">
+        <v>43264</v>
+      </c>
+      <c r="E38" s="12">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F38" s="12">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G38" s="1">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>6</v>
+      </c>
+      <c r="H38" s="1">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="13">
+        <v>43264</v>
+      </c>
+      <c r="E39" s="12">
+        <v>0.76736111111111116</v>
+      </c>
+      <c r="F39" s="12">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="G39" s="1">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>2.3333333333333321</v>
+      </c>
+      <c r="H39" s="1">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="13">
+        <v>43265</v>
+      </c>
+      <c r="E40" s="12">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="F40" s="12">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G40" s="1">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>4.25</v>
+      </c>
+      <c r="H40" s="1">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="13">
+        <v>43266</v>
+      </c>
+      <c r="E41" s="12">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="F41" s="12">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="G41" s="1">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>2.25</v>
+      </c>
+      <c r="H41" s="1">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="13">
+        <v>43267</v>
+      </c>
+      <c r="E42" s="12">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F42" s="12">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G42" s="1">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>4</v>
+      </c>
+      <c r="H42" s="1">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="26">
+        <v>43268</v>
+      </c>
+      <c r="E43" s="27">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F43" s="27">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G43" s="29">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>5.5</v>
+      </c>
+      <c r="H43" s="29">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" s="26">
+        <v>43270</v>
+      </c>
+      <c r="E44" s="27">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F44" s="27">
+        <v>0.5625</v>
+      </c>
+      <c r="G44" s="29">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>4</v>
+      </c>
+      <c r="H44" s="29">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="26">
+        <v>43270</v>
+      </c>
+      <c r="E45" s="27">
+        <v>0.75</v>
+      </c>
+      <c r="F45" s="27">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="G45" s="29">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>5.75</v>
+      </c>
+      <c r="H45" s="29">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46" s="26">
+        <v>43271</v>
+      </c>
+      <c r="E46" s="27">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F46" s="27">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="G46" s="29">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>5.25</v>
+      </c>
+      <c r="H46" s="29">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+      <c r="B47" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D47" s="26">
+        <v>43272</v>
+      </c>
+      <c r="E47" s="27">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="F47" s="27">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="G47" s="29">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>2.25</v>
+      </c>
+      <c r="H47" s="29">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+      <c r="B48" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D48" s="26">
+        <v>43272</v>
+      </c>
+      <c r="E48" s="27">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F48" s="27">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="G48" s="29">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>2.75</v>
+      </c>
+      <c r="H48" s="29">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+      <c r="B49" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D49" s="26">
+        <v>43274</v>
+      </c>
+      <c r="E49" s="27">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F49" s="27">
+        <v>0.875</v>
+      </c>
+      <c r="G49" s="29">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>8</v>
+      </c>
+      <c r="H49" s="29">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+      <c r="B50" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D50" s="26">
+        <v>43276</v>
+      </c>
+      <c r="E50" s="27">
+        <v>0.375</v>
+      </c>
+      <c r="F50" s="27">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G50" s="29">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>7</v>
+      </c>
+      <c r="H50" s="29">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+      <c r="B51" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D51" s="26">
+        <v>43276</v>
+      </c>
+      <c r="E51" s="27">
+        <v>0.8125</v>
+      </c>
+      <c r="F51" s="27">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="G51" s="29">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>4</v>
+      </c>
+      <c r="H51" s="29">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+      <c r="B52" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D52" s="26">
+        <v>43279</v>
+      </c>
+      <c r="E52" s="27">
+        <v>0.375</v>
+      </c>
+      <c r="F52" s="27">
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="G52" s="29">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>6.4166666666666643</v>
+      </c>
+      <c r="H52" s="29">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+      <c r="B53" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D53" s="26">
+        <v>43280</v>
+      </c>
+      <c r="E53" s="27">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="F53" s="27">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="G53" s="29">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>4.5</v>
+      </c>
+      <c r="H53" s="29">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+      <c r="B54" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D54" s="26">
+        <v>43281</v>
+      </c>
+      <c r="E54" s="27">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="F54" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="G54" s="29">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>1.75</v>
+      </c>
+      <c r="H54" s="29">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+      <c r="B55" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D55" s="26">
+        <v>43282</v>
+      </c>
+      <c r="E55" s="27">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="F55" s="27">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="G55" s="29">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>7.5</v>
+      </c>
+      <c r="H55" s="29">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+      <c r="B56" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D56" s="26">
+        <v>43283</v>
+      </c>
+      <c r="E56" s="27">
+        <v>0.65625</v>
+      </c>
+      <c r="F56" s="27">
+        <v>0.96875</v>
+      </c>
+      <c r="G56" s="29">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>7.5</v>
+      </c>
+      <c r="H56" s="29">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+      <c r="B57" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D57" s="26">
+        <v>43285</v>
+      </c>
+      <c r="E57" s="27">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F57" s="27">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="G57" s="29">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>6.25</v>
+      </c>
+      <c r="H57" s="29">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+      <c r="B58" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D58" s="26">
+        <v>43285</v>
+      </c>
+      <c r="E58" s="27">
+        <v>0.75</v>
+      </c>
+      <c r="F58" s="27">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="G58" s="29">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>5.75</v>
+      </c>
+      <c r="H58" s="29">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+      <c r="B59" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D59" s="26">
+        <v>43286</v>
+      </c>
+      <c r="E59" s="27">
+        <v>3.125E-2</v>
+      </c>
+      <c r="F59" s="27">
+        <v>0.19791666666666666</v>
+      </c>
+      <c r="G59" s="29">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+        <v>4</v>
+      </c>
+      <c r="H59" s="29">
+        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="27"/>
+      <c r="F60" s="27"/>
+      <c r="G60" s="29">
+        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
         <v>0</v>
       </c>
-      <c r="H33" s="1">
+      <c r="H60" s="29">
         <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="1">
+    <row r="61" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="27"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="29">
         <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
         <v>0</v>
       </c>
-      <c r="H34" s="1">
+      <c r="H61" s="29">
         <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="1">
+    <row r="62" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="27"/>
+      <c r="F62" s="27"/>
+      <c r="G62" s="29">
         <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
         <v>0</v>
       </c>
-      <c r="H35" s="1">
+      <c r="H62" s="29">
         <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="1">
+    <row r="63" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="27"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="29">
         <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
         <v>0</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H63" s="29">
         <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="1">
+    <row r="64" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="27"/>
+      <c r="F64" s="27"/>
+      <c r="G64" s="29">
         <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
         <v>0</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H64" s="29">
         <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="1">
+    <row r="65" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="26"/>
+      <c r="E65" s="27"/>
+      <c r="F65" s="27"/>
+      <c r="G65" s="29">
         <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
         <v>0</v>
       </c>
-      <c r="H38" s="1">
+      <c r="H65" s="29">
         <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="1">
+    <row r="66" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="1">
         <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
         <v>0</v>
       </c>
-      <c r="H39" s="1">
+      <c r="H66" s="1">
         <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="1">
-        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
+    <row r="67" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+      <c r="B67" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="H40" s="1">
-        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="1">
-        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
-        <v>0</v>
-      </c>
-      <c r="H41" s="1">
-        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="1">
-        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
-        <v>0</v>
-      </c>
-      <c r="H42" s="1">
-        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D43" s="26"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="29">
-        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
-        <v>0</v>
-      </c>
-      <c r="H43" s="29">
-        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D44" s="26"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="29">
-        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
-        <v>0</v>
-      </c>
-      <c r="H44" s="29">
-        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D45" s="26"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="29">
-        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
-        <v>0</v>
-      </c>
-      <c r="H45" s="29">
-        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="3"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="29">
-        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
-        <v>0</v>
-      </c>
-      <c r="H46" s="29">
-        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="3"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="29">
-        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
-        <v>0</v>
-      </c>
-      <c r="H47" s="29">
-        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="3"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="29">
-        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
-        <v>0</v>
-      </c>
-      <c r="H48" s="29">
-        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="3"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="29">
-        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
-        <v>0</v>
-      </c>
-      <c r="H49" s="29">
-        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="3"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="1">
-        <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
-        <v>0</v>
-      </c>
-      <c r="H50" s="1">
-        <f>WEEKNUM(Tabelle36[[#This Row],[Datum]],2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="3"/>
-      <c r="B51" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
-      <c r="G51" s="1">
-        <f>SUM(G7:G50)</f>
-        <v>65.75</v>
-      </c>
-      <c r="H51" s="1"/>
-    </row>
-    <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="3"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-    </row>
-    <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-    </row>
-    <row r="54" spans="1:8" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A54" s="3"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-    </row>
-    <row r="55" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-    </row>
-    <row r="56" spans="1:8" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="3"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="5"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-    </row>
-    <row r="57" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="4"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-    </row>
-    <row r="58" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="4"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-    </row>
-    <row r="59" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="4"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-    </row>
-    <row r="60" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="4"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-    </row>
-    <row r="61" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="4"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-    </row>
-    <row r="62" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="4"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-    </row>
-    <row r="63" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="4"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-    </row>
-    <row r="64" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="3"/>
-      <c r="B64" s="9"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="4"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-    </row>
-    <row r="65" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="4"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-    </row>
-    <row r="66" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="4"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-    </row>
-    <row r="67" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="4"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="1">
+        <f>SUM(G7:G66)</f>
+        <v>199.24999999999997</v>
+      </c>
       <c r="H67" s="1"/>
     </row>
-    <row r="68" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="4"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
-      <c r="D69" s="4"/>
+      <c r="D69" s="3"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
+      <c r="B70" s="7"/>
       <c r="C70" s="3"/>
-      <c r="D70" s="4"/>
+      <c r="D70" s="3"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
     </row>
-    <row r="71" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
-      <c r="D71" s="4"/>
+      <c r="D71" s="3"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
     </row>
-    <row r="72" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="4"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="5"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
     </row>
-    <row r="73" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -1840,7 +2331,7 @@
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -1849,7 +2340,7 @@
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -1858,7 +2349,7 @@
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -1867,7 +2358,7 @@
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
     </row>
-    <row r="77" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -1876,7 +2367,7 @@
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
     </row>
-    <row r="78" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -1885,7 +2376,7 @@
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
     </row>
-    <row r="79" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -1894,16 +2385,16 @@
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
     </row>
-    <row r="80" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
+      <c r="B80" s="9"/>
       <c r="C80" s="3"/>
       <c r="D80" s="4"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
     </row>
-    <row r="81" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -1912,7 +2403,7 @@
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -1921,7 +2412,7 @@
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
     </row>
-    <row r="83" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -1930,7 +2421,7 @@
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
     </row>
-    <row r="84" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -1939,7 +2430,7 @@
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
     </row>
-    <row r="85" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -1948,7 +2439,7 @@
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
     </row>
-    <row r="86" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -1957,7 +2448,7 @@
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
     </row>
-    <row r="87" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -1966,7 +2457,7 @@
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -1975,7 +2466,7 @@
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
     </row>
-    <row r="89" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -1984,7 +2475,7 @@
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
     </row>
-    <row r="90" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -1993,7 +2484,7 @@
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
     </row>
-    <row r="91" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -2002,7 +2493,7 @@
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
     </row>
-    <row r="92" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -2011,7 +2502,7 @@
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
     </row>
-    <row r="93" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -2020,7 +2511,7 @@
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
     </row>
-    <row r="94" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -2029,7 +2520,7 @@
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
     </row>
-    <row r="95" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -2038,61 +2529,61 @@
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
     </row>
-    <row r="96" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
-      <c r="B96" s="8"/>
+      <c r="B96" s="3"/>
       <c r="C96" s="3"/>
       <c r="D96" s="4"/>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
     </row>
-    <row r="97" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
-      <c r="D97" s="3"/>
+      <c r="D97" s="4"/>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
     </row>
-    <row r="98" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
+      <c r="D98" s="4"/>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
     </row>
-    <row r="99" spans="1:8" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
-      <c r="B99" s="7"/>
+      <c r="B99" s="3"/>
       <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
+      <c r="D99" s="4"/>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
     </row>
-    <row r="100" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
+      <c r="D100" s="4"/>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
     </row>
-    <row r="101" spans="1:8" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
-      <c r="B101" s="6"/>
-      <c r="C101" s="6"/>
-      <c r="D101" s="5"/>
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="4"/>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
     </row>
-    <row r="102" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -2101,7 +2592,7 @@
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
     </row>
-    <row r="103" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -2110,7 +2601,7 @@
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
     </row>
-    <row r="104" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -2119,7 +2610,7 @@
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
     </row>
-    <row r="105" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -2128,7 +2619,7 @@
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
     </row>
-    <row r="106" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -2137,7 +2628,7 @@
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
     </row>
-    <row r="107" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -2146,7 +2637,7 @@
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
     </row>
-    <row r="108" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -2155,7 +2646,7 @@
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
     </row>
-    <row r="109" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -2164,7 +2655,7 @@
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
     </row>
-    <row r="110" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -2173,7 +2664,7 @@
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
     </row>
-    <row r="111" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -2182,61 +2673,61 @@
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
     </row>
-    <row r="112" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
-      <c r="B112" s="3"/>
+      <c r="B112" s="8"/>
       <c r="C112" s="3"/>
       <c r="D112" s="4"/>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
     </row>
-    <row r="113" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
-      <c r="D113" s="4"/>
+      <c r="D113" s="3"/>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
     </row>
-    <row r="114" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
-      <c r="D114" s="4"/>
+      <c r="D114" s="3"/>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
       <c r="H114" s="1"/>
     </row>
-    <row r="115" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A115" s="3"/>
-      <c r="B115" s="3"/>
+      <c r="B115" s="7"/>
       <c r="C115" s="3"/>
-      <c r="D115" s="4"/>
+      <c r="D115" s="3"/>
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
     </row>
-    <row r="116" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
-      <c r="D116" s="4"/>
+      <c r="D116" s="3"/>
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
     </row>
-    <row r="117" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
-      <c r="B117" s="3"/>
-      <c r="C117" s="3"/>
-      <c r="D117" s="4"/>
+      <c r="B117" s="6"/>
+      <c r="C117" s="6"/>
+      <c r="D117" s="5"/>
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
     </row>
-    <row r="118" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
@@ -2245,7 +2736,7 @@
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
     </row>
-    <row r="119" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -2254,7 +2745,7 @@
       <c r="G119" s="1"/>
       <c r="H119" s="1"/>
     </row>
-    <row r="120" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -2263,7 +2754,7 @@
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
     </row>
-    <row r="121" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -2272,7 +2763,7 @@
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
     </row>
-    <row r="122" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -2281,7 +2772,7 @@
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
     </row>
-    <row r="123" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -2290,7 +2781,7 @@
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
     </row>
-    <row r="124" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -2299,7 +2790,7 @@
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
     </row>
-    <row r="125" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -2308,7 +2799,7 @@
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
     </row>
-    <row r="126" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -2317,7 +2808,7 @@
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
     </row>
-    <row r="127" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -2326,7 +2817,7 @@
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
     </row>
-    <row r="128" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -2335,7 +2826,7 @@
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
     </row>
-    <row r="129" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -2344,7 +2835,7 @@
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
     </row>
-    <row r="130" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
@@ -2353,7 +2844,7 @@
       <c r="G130" s="1"/>
       <c r="H130" s="1"/>
     </row>
-    <row r="131" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
@@ -2362,7 +2853,7 @@
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
     </row>
-    <row r="132" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
@@ -2371,7 +2862,7 @@
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
     </row>
-    <row r="133" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
@@ -2380,7 +2871,7 @@
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
     </row>
-    <row r="134" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
@@ -2389,7 +2880,7 @@
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
     </row>
-    <row r="135" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
@@ -2398,7 +2889,7 @@
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
     </row>
-    <row r="136" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
@@ -2407,7 +2898,7 @@
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
     </row>
-    <row r="137" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
@@ -2416,7 +2907,7 @@
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
     </row>
-    <row r="138" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
@@ -2425,7 +2916,7 @@
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
     </row>
-    <row r="139" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
@@ -2434,7 +2925,7 @@
       <c r="G139" s="1"/>
       <c r="H139" s="1"/>
     </row>
-    <row r="140" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
@@ -2443,61 +2934,61 @@
       <c r="G140" s="1"/>
       <c r="H140" s="1"/>
     </row>
-    <row r="141" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
-      <c r="B141" s="8"/>
+      <c r="B141" s="3"/>
       <c r="C141" s="3"/>
       <c r="D141" s="4"/>
       <c r="F141" s="1"/>
       <c r="G141" s="1"/>
       <c r="H141" s="1"/>
     </row>
-    <row r="142" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
-      <c r="D142" s="3"/>
+      <c r="D142" s="4"/>
       <c r="F142" s="1"/>
       <c r="G142" s="1"/>
       <c r="H142" s="1"/>
     </row>
-    <row r="143" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="3"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
-      <c r="D143" s="3"/>
+      <c r="D143" s="4"/>
       <c r="F143" s="1"/>
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
     </row>
-    <row r="144" spans="1:8" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3"/>
-      <c r="B144" s="7"/>
+      <c r="B144" s="3"/>
       <c r="C144" s="3"/>
-      <c r="D144" s="3"/>
+      <c r="D144" s="4"/>
       <c r="F144" s="1"/>
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
     </row>
-    <row r="145" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="3"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
-      <c r="D145" s="3"/>
+      <c r="D145" s="4"/>
       <c r="F145" s="1"/>
       <c r="G145" s="1"/>
       <c r="H145" s="1"/>
     </row>
-    <row r="146" spans="1:8" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3"/>
-      <c r="B146" s="6"/>
-      <c r="C146" s="6"/>
-      <c r="D146" s="5"/>
+      <c r="B146" s="3"/>
+      <c r="C146" s="3"/>
+      <c r="D146" s="4"/>
       <c r="F146" s="1"/>
       <c r="G146" s="1"/>
       <c r="H146" s="1"/>
     </row>
-    <row r="147" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
@@ -2506,7 +2997,7 @@
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
     </row>
-    <row r="148" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
@@ -2515,7 +3006,7 @@
       <c r="G148" s="1"/>
       <c r="H148" s="1"/>
     </row>
-    <row r="149" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="3"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
@@ -2524,7 +3015,7 @@
       <c r="G149" s="1"/>
       <c r="H149" s="1"/>
     </row>
-    <row r="150" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
@@ -2533,7 +3024,7 @@
       <c r="G150" s="1"/>
       <c r="H150" s="1"/>
     </row>
-    <row r="151" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
@@ -2542,7 +3033,7 @@
       <c r="G151" s="1"/>
       <c r="H151" s="1"/>
     </row>
-    <row r="152" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
@@ -2551,7 +3042,7 @@
       <c r="G152" s="1"/>
       <c r="H152" s="1"/>
     </row>
-    <row r="153" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="3"/>
       <c r="C153" s="3"/>
@@ -2560,7 +3051,7 @@
       <c r="G153" s="1"/>
       <c r="H153" s="1"/>
     </row>
-    <row r="154" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
@@ -2569,7 +3060,7 @@
       <c r="G154" s="1"/>
       <c r="H154" s="1"/>
     </row>
-    <row r="155" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
@@ -2578,7 +3069,7 @@
       <c r="G155" s="1"/>
       <c r="H155" s="1"/>
     </row>
-    <row r="156" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3"/>
       <c r="B156" s="3"/>
       <c r="C156" s="3"/>
@@ -2587,61 +3078,61 @@
       <c r="G156" s="1"/>
       <c r="H156" s="1"/>
     </row>
-    <row r="157" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="3"/>
-      <c r="B157" s="3"/>
+      <c r="B157" s="8"/>
       <c r="C157" s="3"/>
       <c r="D157" s="4"/>
       <c r="F157" s="1"/>
       <c r="G157" s="1"/>
       <c r="H157" s="1"/>
     </row>
-    <row r="158" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="3"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
-      <c r="D158" s="4"/>
+      <c r="D158" s="3"/>
       <c r="F158" s="1"/>
       <c r="G158" s="1"/>
       <c r="H158" s="1"/>
     </row>
-    <row r="159" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="3"/>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
-      <c r="D159" s="4"/>
+      <c r="D159" s="3"/>
       <c r="F159" s="1"/>
       <c r="G159" s="1"/>
       <c r="H159" s="1"/>
     </row>
-    <row r="160" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A160" s="3"/>
-      <c r="B160" s="3"/>
+      <c r="B160" s="7"/>
       <c r="C160" s="3"/>
-      <c r="D160" s="4"/>
+      <c r="D160" s="3"/>
       <c r="F160" s="1"/>
       <c r="G160" s="1"/>
       <c r="H160" s="1"/>
     </row>
-    <row r="161" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3"/>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
-      <c r="D161" s="4"/>
+      <c r="D161" s="3"/>
       <c r="F161" s="1"/>
       <c r="G161" s="1"/>
       <c r="H161" s="1"/>
     </row>
-    <row r="162" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A162" s="3"/>
-      <c r="B162" s="3"/>
-      <c r="C162" s="3"/>
-      <c r="D162" s="4"/>
+      <c r="B162" s="6"/>
+      <c r="C162" s="6"/>
+      <c r="D162" s="5"/>
       <c r="F162" s="1"/>
       <c r="G162" s="1"/>
       <c r="H162" s="1"/>
     </row>
-    <row r="163" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="3"/>
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
@@ -2650,7 +3141,7 @@
       <c r="G163" s="1"/>
       <c r="H163" s="1"/>
     </row>
-    <row r="164" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3"/>
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
@@ -2659,7 +3150,7 @@
       <c r="G164" s="1"/>
       <c r="H164" s="1"/>
     </row>
-    <row r="165" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3"/>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
@@ -2668,7 +3159,7 @@
       <c r="G165" s="1"/>
       <c r="H165" s="1"/>
     </row>
-    <row r="166" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3"/>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
@@ -2677,7 +3168,7 @@
       <c r="G166" s="1"/>
       <c r="H166" s="1"/>
     </row>
-    <row r="167" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="3"/>
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
@@ -2686,7 +3177,7 @@
       <c r="G167" s="1"/>
       <c r="H167" s="1"/>
     </row>
-    <row r="168" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="3"/>
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
@@ -2695,7 +3186,7 @@
       <c r="G168" s="1"/>
       <c r="H168" s="1"/>
     </row>
-    <row r="169" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="3"/>
       <c r="B169" s="3"/>
       <c r="C169" s="3"/>
@@ -2704,7 +3195,7 @@
       <c r="G169" s="1"/>
       <c r="H169" s="1"/>
     </row>
-    <row r="170" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3"/>
       <c r="B170" s="3"/>
       <c r="C170" s="3"/>
@@ -2713,7 +3204,7 @@
       <c r="G170" s="1"/>
       <c r="H170" s="1"/>
     </row>
-    <row r="171" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="3"/>
       <c r="B171" s="3"/>
       <c r="C171" s="3"/>
@@ -2722,7 +3213,7 @@
       <c r="G171" s="1"/>
       <c r="H171" s="1"/>
     </row>
-    <row r="172" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="3"/>
       <c r="B172" s="3"/>
       <c r="C172" s="3"/>
@@ -2731,7 +3222,7 @@
       <c r="G172" s="1"/>
       <c r="H172" s="1"/>
     </row>
-    <row r="173" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="3"/>
       <c r="B173" s="3"/>
       <c r="C173" s="3"/>
@@ -2740,7 +3231,7 @@
       <c r="G173" s="1"/>
       <c r="H173" s="1"/>
     </row>
-    <row r="174" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="3"/>
       <c r="B174" s="3"/>
       <c r="C174" s="3"/>
@@ -2749,7 +3240,7 @@
       <c r="G174" s="1"/>
       <c r="H174" s="1"/>
     </row>
-    <row r="175" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="3"/>
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
@@ -2758,7 +3249,7 @@
       <c r="G175" s="1"/>
       <c r="H175" s="1"/>
     </row>
-    <row r="176" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="3"/>
       <c r="B176" s="3"/>
       <c r="C176" s="3"/>
@@ -2767,7 +3258,7 @@
       <c r="G176" s="1"/>
       <c r="H176" s="1"/>
     </row>
-    <row r="177" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="3"/>
       <c r="B177" s="3"/>
       <c r="C177" s="3"/>
@@ -2776,7 +3267,7 @@
       <c r="G177" s="1"/>
       <c r="H177" s="1"/>
     </row>
-    <row r="178" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="3"/>
       <c r="B178" s="3"/>
       <c r="C178" s="3"/>
@@ -2785,7 +3276,7 @@
       <c r="G178" s="1"/>
       <c r="H178" s="1"/>
     </row>
-    <row r="179" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="3"/>
       <c r="B179" s="3"/>
       <c r="C179" s="3"/>
@@ -2794,7 +3285,7 @@
       <c r="G179" s="1"/>
       <c r="H179" s="1"/>
     </row>
-    <row r="180" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="3"/>
       <c r="B180" s="3"/>
       <c r="C180" s="3"/>
@@ -2803,7 +3294,7 @@
       <c r="G180" s="1"/>
       <c r="H180" s="1"/>
     </row>
-    <row r="181" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="3"/>
       <c r="B181" s="3"/>
       <c r="C181" s="3"/>
@@ -2812,7 +3303,7 @@
       <c r="G181" s="1"/>
       <c r="H181" s="1"/>
     </row>
-    <row r="182" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="3"/>
       <c r="B182" s="3"/>
       <c r="C182" s="3"/>
@@ -2821,7 +3312,7 @@
       <c r="G182" s="1"/>
       <c r="H182" s="1"/>
     </row>
-    <row r="183" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="3"/>
       <c r="B183" s="3"/>
       <c r="C183" s="3"/>
@@ -2830,7 +3321,7 @@
       <c r="G183" s="1"/>
       <c r="H183" s="1"/>
     </row>
-    <row r="184" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="3"/>
       <c r="B184" s="3"/>
       <c r="C184" s="3"/>
@@ -2839,7 +3330,7 @@
       <c r="G184" s="1"/>
       <c r="H184" s="1"/>
     </row>
-    <row r="185" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="3"/>
       <c r="B185" s="3"/>
       <c r="C185" s="3"/>
@@ -2848,61 +3339,61 @@
       <c r="G185" s="1"/>
       <c r="H185" s="1"/>
     </row>
-    <row r="186" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="3"/>
-      <c r="B186" s="8"/>
+      <c r="B186" s="3"/>
       <c r="C186" s="3"/>
       <c r="D186" s="4"/>
       <c r="F186" s="1"/>
       <c r="G186" s="1"/>
       <c r="H186" s="1"/>
     </row>
-    <row r="187" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="3"/>
       <c r="B187" s="3"/>
       <c r="C187" s="3"/>
-      <c r="D187" s="3"/>
+      <c r="D187" s="4"/>
       <c r="F187" s="1"/>
       <c r="G187" s="1"/>
       <c r="H187" s="1"/>
     </row>
-    <row r="188" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="3"/>
       <c r="B188" s="3"/>
       <c r="C188" s="3"/>
-      <c r="D188" s="3"/>
+      <c r="D188" s="4"/>
       <c r="F188" s="1"/>
       <c r="G188" s="1"/>
       <c r="H188" s="1"/>
     </row>
-    <row r="189" spans="1:8" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="3"/>
-      <c r="B189" s="7"/>
+      <c r="B189" s="3"/>
       <c r="C189" s="3"/>
-      <c r="D189" s="3"/>
+      <c r="D189" s="4"/>
       <c r="F189" s="1"/>
       <c r="G189" s="1"/>
       <c r="H189" s="1"/>
     </row>
-    <row r="190" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" s="3"/>
       <c r="B190" s="3"/>
       <c r="C190" s="3"/>
-      <c r="D190" s="3"/>
+      <c r="D190" s="4"/>
       <c r="F190" s="1"/>
       <c r="G190" s="1"/>
       <c r="H190" s="1"/>
     </row>
-    <row r="191" spans="1:8" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="3"/>
-      <c r="B191" s="6"/>
-      <c r="C191" s="6"/>
-      <c r="D191" s="5"/>
+      <c r="B191" s="3"/>
+      <c r="C191" s="3"/>
+      <c r="D191" s="4"/>
       <c r="F191" s="1"/>
       <c r="G191" s="1"/>
       <c r="H191" s="1"/>
     </row>
-    <row r="192" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="3"/>
       <c r="B192" s="3"/>
       <c r="C192" s="3"/>
@@ -2911,7 +3402,7 @@
       <c r="G192" s="1"/>
       <c r="H192" s="1"/>
     </row>
-    <row r="193" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="3"/>
       <c r="B193" s="3"/>
       <c r="C193" s="3"/>
@@ -2920,7 +3411,7 @@
       <c r="G193" s="1"/>
       <c r="H193" s="1"/>
     </row>
-    <row r="194" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="3"/>
       <c r="B194" s="3"/>
       <c r="C194" s="3"/>
@@ -2929,7 +3420,7 @@
       <c r="G194" s="1"/>
       <c r="H194" s="1"/>
     </row>
-    <row r="195" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="3"/>
       <c r="B195" s="3"/>
       <c r="C195" s="3"/>
@@ -2938,7 +3429,7 @@
       <c r="G195" s="1"/>
       <c r="H195" s="1"/>
     </row>
-    <row r="196" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="3"/>
       <c r="B196" s="3"/>
       <c r="C196" s="3"/>
@@ -2947,7 +3438,7 @@
       <c r="G196" s="1"/>
       <c r="H196" s="1"/>
     </row>
-    <row r="197" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="3"/>
       <c r="B197" s="3"/>
       <c r="C197" s="3"/>
@@ -2956,7 +3447,7 @@
       <c r="G197" s="1"/>
       <c r="H197" s="1"/>
     </row>
-    <row r="198" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="3"/>
       <c r="B198" s="3"/>
       <c r="C198" s="3"/>
@@ -2965,7 +3456,7 @@
       <c r="G198" s="1"/>
       <c r="H198" s="1"/>
     </row>
-    <row r="199" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A199" s="3"/>
       <c r="B199" s="3"/>
       <c r="C199" s="3"/>
@@ -2974,7 +3465,7 @@
       <c r="G199" s="1"/>
       <c r="H199" s="1"/>
     </row>
-    <row r="200" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A200" s="3"/>
       <c r="B200" s="3"/>
       <c r="C200" s="3"/>
@@ -2983,7 +3474,7 @@
       <c r="G200" s="1"/>
       <c r="H200" s="1"/>
     </row>
-    <row r="201" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A201" s="3"/>
       <c r="B201" s="3"/>
       <c r="C201" s="3"/>
@@ -2992,61 +3483,61 @@
       <c r="G201" s="1"/>
       <c r="H201" s="1"/>
     </row>
-    <row r="202" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A202" s="3"/>
-      <c r="B202" s="3"/>
+      <c r="B202" s="8"/>
       <c r="C202" s="3"/>
       <c r="D202" s="4"/>
       <c r="F202" s="1"/>
       <c r="G202" s="1"/>
       <c r="H202" s="1"/>
     </row>
-    <row r="203" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A203" s="3"/>
       <c r="B203" s="3"/>
       <c r="C203" s="3"/>
-      <c r="D203" s="4"/>
+      <c r="D203" s="3"/>
       <c r="F203" s="1"/>
       <c r="G203" s="1"/>
       <c r="H203" s="1"/>
     </row>
-    <row r="204" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A204" s="3"/>
       <c r="B204" s="3"/>
       <c r="C204" s="3"/>
-      <c r="D204" s="4"/>
+      <c r="D204" s="3"/>
       <c r="F204" s="1"/>
       <c r="G204" s="1"/>
       <c r="H204" s="1"/>
     </row>
-    <row r="205" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:8" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A205" s="3"/>
-      <c r="B205" s="3"/>
+      <c r="B205" s="7"/>
       <c r="C205" s="3"/>
-      <c r="D205" s="4"/>
+      <c r="D205" s="3"/>
       <c r="F205" s="1"/>
       <c r="G205" s="1"/>
       <c r="H205" s="1"/>
     </row>
-    <row r="206" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A206" s="3"/>
       <c r="B206" s="3"/>
       <c r="C206" s="3"/>
-      <c r="D206" s="4"/>
+      <c r="D206" s="3"/>
       <c r="F206" s="1"/>
       <c r="G206" s="1"/>
       <c r="H206" s="1"/>
     </row>
-    <row r="207" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A207" s="3"/>
-      <c r="B207" s="3"/>
-      <c r="C207" s="3"/>
-      <c r="D207" s="4"/>
+      <c r="B207" s="6"/>
+      <c r="C207" s="6"/>
+      <c r="D207" s="5"/>
       <c r="F207" s="1"/>
       <c r="G207" s="1"/>
       <c r="H207" s="1"/>
     </row>
-    <row r="208" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A208" s="3"/>
       <c r="B208" s="3"/>
       <c r="C208" s="3"/>
@@ -3055,7 +3546,7 @@
       <c r="G208" s="1"/>
       <c r="H208" s="1"/>
     </row>
-    <row r="209" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A209" s="3"/>
       <c r="B209" s="3"/>
       <c r="C209" s="3"/>
@@ -3064,7 +3555,7 @@
       <c r="G209" s="1"/>
       <c r="H209" s="1"/>
     </row>
-    <row r="210" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A210" s="3"/>
       <c r="B210" s="3"/>
       <c r="C210" s="3"/>
@@ -3073,7 +3564,7 @@
       <c r="G210" s="1"/>
       <c r="H210" s="1"/>
     </row>
-    <row r="211" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A211" s="3"/>
       <c r="B211" s="3"/>
       <c r="C211" s="3"/>
@@ -3082,7 +3573,7 @@
       <c r="G211" s="1"/>
       <c r="H211" s="1"/>
     </row>
-    <row r="212" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A212" s="3"/>
       <c r="B212" s="3"/>
       <c r="C212" s="3"/>
@@ -3091,7 +3582,7 @@
       <c r="G212" s="1"/>
       <c r="H212" s="1"/>
     </row>
-    <row r="213" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A213" s="3"/>
       <c r="B213" s="3"/>
       <c r="C213" s="3"/>
@@ -3100,7 +3591,7 @@
       <c r="G213" s="1"/>
       <c r="H213" s="1"/>
     </row>
-    <row r="214" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A214" s="3"/>
       <c r="B214" s="3"/>
       <c r="C214" s="3"/>
@@ -3109,7 +3600,7 @@
       <c r="G214" s="1"/>
       <c r="H214" s="1"/>
     </row>
-    <row r="215" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A215" s="3"/>
       <c r="B215" s="3"/>
       <c r="C215" s="3"/>
@@ -3118,7 +3609,7 @@
       <c r="G215" s="1"/>
       <c r="H215" s="1"/>
     </row>
-    <row r="216" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A216" s="3"/>
       <c r="B216" s="3"/>
       <c r="C216" s="3"/>
@@ -3127,7 +3618,7 @@
       <c r="G216" s="1"/>
       <c r="H216" s="1"/>
     </row>
-    <row r="217" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A217" s="3"/>
       <c r="B217" s="3"/>
       <c r="C217" s="3"/>
@@ -3136,7 +3627,7 @@
       <c r="G217" s="1"/>
       <c r="H217" s="1"/>
     </row>
-    <row r="218" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A218" s="3"/>
       <c r="B218" s="3"/>
       <c r="C218" s="3"/>
@@ -3145,7 +3636,7 @@
       <c r="G218" s="1"/>
       <c r="H218" s="1"/>
     </row>
-    <row r="219" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="3"/>
       <c r="B219" s="3"/>
       <c r="C219" s="3"/>
@@ -3154,7 +3645,7 @@
       <c r="G219" s="1"/>
       <c r="H219" s="1"/>
     </row>
-    <row r="220" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A220" s="3"/>
       <c r="B220" s="3"/>
       <c r="C220" s="3"/>
@@ -3163,7 +3654,7 @@
       <c r="G220" s="1"/>
       <c r="H220" s="1"/>
     </row>
-    <row r="221" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A221" s="3"/>
       <c r="B221" s="3"/>
       <c r="C221" s="3"/>
@@ -3172,7 +3663,7 @@
       <c r="G221" s="1"/>
       <c r="H221" s="1"/>
     </row>
-    <row r="222" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" s="3"/>
       <c r="B222" s="3"/>
       <c r="C222" s="3"/>
@@ -3181,41 +3672,184 @@
       <c r="G222" s="1"/>
       <c r="H222" s="1"/>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="3"/>
       <c r="B223" s="3"/>
       <c r="C223" s="3"/>
       <c r="D223" s="4"/>
-    </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F223" s="1"/>
+      <c r="G223" s="1"/>
+      <c r="H223" s="1"/>
+    </row>
+    <row r="224" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A224" s="3"/>
       <c r="B224" s="3"/>
       <c r="C224" s="3"/>
       <c r="D224" s="4"/>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F224" s="1"/>
+      <c r="G224" s="1"/>
+      <c r="H224" s="1"/>
+    </row>
+    <row r="225" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A225" s="3"/>
       <c r="B225" s="3"/>
       <c r="C225" s="3"/>
       <c r="D225" s="4"/>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F225" s="1"/>
+      <c r="G225" s="1"/>
+      <c r="H225" s="1"/>
+    </row>
+    <row r="226" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A226" s="3"/>
       <c r="B226" s="3"/>
       <c r="C226" s="3"/>
       <c r="D226" s="4"/>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F226" s="1"/>
+      <c r="G226" s="1"/>
+      <c r="H226" s="1"/>
+    </row>
+    <row r="227" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A227" s="3"/>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B227" s="3"/>
+      <c r="C227" s="3"/>
+      <c r="D227" s="4"/>
+      <c r="F227" s="1"/>
+      <c r="G227" s="1"/>
+      <c r="H227" s="1"/>
+    </row>
+    <row r="228" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A228" s="3"/>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B228" s="3"/>
+      <c r="C228" s="3"/>
+      <c r="D228" s="4"/>
+      <c r="F228" s="1"/>
+      <c r="G228" s="1"/>
+      <c r="H228" s="1"/>
+    </row>
+    <row r="229" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A229" s="3"/>
+      <c r="B229" s="3"/>
+      <c r="C229" s="3"/>
+      <c r="D229" s="4"/>
+      <c r="F229" s="1"/>
+      <c r="G229" s="1"/>
+      <c r="H229" s="1"/>
+    </row>
+    <row r="230" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="3"/>
+      <c r="B230" s="3"/>
+      <c r="C230" s="3"/>
+      <c r="D230" s="4"/>
+      <c r="F230" s="1"/>
+      <c r="G230" s="1"/>
+      <c r="H230" s="1"/>
+    </row>
+    <row r="231" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="3"/>
+      <c r="B231" s="3"/>
+      <c r="C231" s="3"/>
+      <c r="D231" s="4"/>
+      <c r="F231" s="1"/>
+      <c r="G231" s="1"/>
+      <c r="H231" s="1"/>
+    </row>
+    <row r="232" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="3"/>
+      <c r="B232" s="3"/>
+      <c r="C232" s="3"/>
+      <c r="D232" s="4"/>
+      <c r="F232" s="1"/>
+      <c r="G232" s="1"/>
+      <c r="H232" s="1"/>
+    </row>
+    <row r="233" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="3"/>
+      <c r="B233" s="3"/>
+      <c r="C233" s="3"/>
+      <c r="D233" s="4"/>
+      <c r="F233" s="1"/>
+      <c r="G233" s="1"/>
+      <c r="H233" s="1"/>
+    </row>
+    <row r="234" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="3"/>
+      <c r="B234" s="3"/>
+      <c r="C234" s="3"/>
+      <c r="D234" s="4"/>
+      <c r="F234" s="1"/>
+      <c r="G234" s="1"/>
+      <c r="H234" s="1"/>
+    </row>
+    <row r="235" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="3"/>
+      <c r="B235" s="3"/>
+      <c r="C235" s="3"/>
+      <c r="D235" s="4"/>
+      <c r="F235" s="1"/>
+      <c r="G235" s="1"/>
+      <c r="H235" s="1"/>
+    </row>
+    <row r="236" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="3"/>
+      <c r="B236" s="3"/>
+      <c r="C236" s="3"/>
+      <c r="D236" s="4"/>
+      <c r="F236" s="1"/>
+      <c r="G236" s="1"/>
+      <c r="H236" s="1"/>
+    </row>
+    <row r="237" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="3"/>
+      <c r="B237" s="3"/>
+      <c r="C237" s="3"/>
+      <c r="D237" s="4"/>
+      <c r="F237" s="1"/>
+      <c r="G237" s="1"/>
+      <c r="H237" s="1"/>
+    </row>
+    <row r="238" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="3"/>
+      <c r="B238" s="3"/>
+      <c r="C238" s="3"/>
+      <c r="D238" s="4"/>
+      <c r="F238" s="1"/>
+      <c r="G238" s="1"/>
+      <c r="H238" s="1"/>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A239" s="3"/>
+      <c r="B239" s="3"/>
+      <c r="C239" s="3"/>
+      <c r="D239" s="4"/>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A240" s="3"/>
+      <c r="B240" s="3"/>
+      <c r="C240" s="3"/>
+      <c r="D240" s="4"/>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" s="3"/>
+      <c r="B241" s="3"/>
+      <c r="C241" s="3"/>
+      <c r="D241" s="4"/>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" s="3"/>
+      <c r="B242" s="3"/>
+      <c r="C242" s="3"/>
+      <c r="D242" s="4"/>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" s="3"/>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" s="3"/>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>